<commit_message>
Correction of English text. Correction mistakes. Added css for exercises. Add favicon.
</commit_message>
<xml_diff>
--- a/data/Car.xlsx
+++ b/data/Car.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\studieboeken\learnexcel\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD3D852-6D85-454D-B242-540584C02B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="14520" windowHeight="12855"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -583,23 +589,23 @@
     <t>Top Speed</t>
   </si>
   <si>
-    <t>Super</t>
-  </si>
-  <si>
-    <t>Ordinary</t>
-  </si>
-  <si>
     <t>Diesel</t>
+  </si>
+  <si>
+    <t>Regular</t>
+  </si>
+  <si>
+    <t>Premium</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -641,7 +647,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -649,18 +655,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Valuta" xfId="1" builtinId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -668,14 +674,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -713,7 +722,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -785,7 +794,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -958,11 +967,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
@@ -1013,7 +1022,7 @@
         <v>170</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F2" s="3">
         <v>12.2</v>
@@ -1036,7 +1045,7 @@
         <v>190</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F3" s="3">
         <v>10</v>
@@ -1059,7 +1068,7 @@
         <v>175</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F4" s="3">
         <v>12.9</v>
@@ -1082,7 +1091,7 @@
         <v>190</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F5" s="3">
         <v>10.1</v>
@@ -1128,7 +1137,7 @@
         <v>153</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F7" s="3">
         <v>16.2</v>
@@ -1174,7 +1183,7 @@
         <v>158</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F9" s="3">
         <v>14.9</v>
@@ -1220,7 +1229,7 @@
         <v>138</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F11" s="3">
         <v>14.4</v>
@@ -1243,7 +1252,7 @@
         <v>155</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F12" s="3">
         <v>13.2</v>
@@ -1266,7 +1275,7 @@
         <v>154</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F13" s="3">
         <v>13.2</v>
@@ -1289,7 +1298,7 @@
         <v>175</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F14" s="3">
         <v>11.6</v>
@@ -1312,7 +1321,7 @@
         <v>184</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F15" s="3">
         <v>11.2</v>
@@ -1335,7 +1344,7 @@
         <v>217</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F16" s="3">
         <v>9.9</v>
@@ -1358,7 +1367,7 @@
         <v>175</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F17" s="3">
         <v>10.4</v>
@@ -1381,7 +1390,7 @@
         <v>185</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F18" s="3">
         <v>10.3</v>
@@ -1404,7 +1413,7 @@
         <v>185</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F19" s="3">
         <v>9.4</v>
@@ -1450,7 +1459,7 @@
         <v>115</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F21" s="3">
         <v>16.5</v>
@@ -1473,7 +1482,7 @@
         <v>124</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F22" s="3">
         <v>15.1</v>
@@ -1496,7 +1505,7 @@
         <v>150</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F23" s="3">
         <v>12.1</v>
@@ -1519,7 +1528,7 @@
         <v>155</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F24" s="3">
         <v>14.2</v>
@@ -1542,7 +1551,7 @@
         <v>176</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F25" s="3">
         <v>10.199999999999999</v>
@@ -1565,7 +1574,7 @@
         <v>186</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F26" s="3">
         <v>10.4</v>
@@ -1588,7 +1597,7 @@
         <v>149</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F27" s="3">
         <v>12.1</v>
@@ -1657,7 +1666,7 @@
         <v>125</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F30" s="3">
         <v>17.8</v>
@@ -1703,7 +1712,7 @@
         <v>125</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F32" s="3">
         <v>16.100000000000001</v>
@@ -1726,7 +1735,7 @@
         <v>145</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F33" s="3">
         <v>16.3</v>
@@ -1749,7 +1758,7 @@
         <v>155</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F34" s="3">
         <v>18.600000000000001</v>
@@ -1772,7 +1781,7 @@
         <v>150</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F35" s="3">
         <v>13.4</v>
@@ -1795,7 +1804,7 @@
         <v>150</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F36" s="3">
         <v>15.2</v>
@@ -1818,7 +1827,7 @@
         <v>155</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F37" s="3">
         <v>13.4</v>
@@ -1841,7 +1850,7 @@
         <v>150</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F38" s="3">
         <v>13.6</v>
@@ -1864,7 +1873,7 @@
         <v>180</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F39" s="3">
         <v>13.7</v>
@@ -1887,7 +1896,7 @@
         <v>185</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F40" s="3">
         <v>14.1</v>
@@ -1910,7 +1919,7 @@
         <v>136</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F41" s="3">
         <v>13.6</v>
@@ -1933,7 +1942,7 @@
         <v>148</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F42" s="3">
         <v>15.9</v>
@@ -1956,7 +1965,7 @@
         <v>144</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F43" s="3">
         <v>14.1</v>
@@ -1979,7 +1988,7 @@
         <v>150</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F44" s="3">
         <v>16.899999999999999</v>
@@ -2002,7 +2011,7 @@
         <v>167</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F45" s="3">
         <v>14.7</v>
@@ -2025,7 +2034,7 @@
         <v>165</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F46" s="3">
         <v>18.3</v>
@@ -2048,7 +2057,7 @@
         <v>165</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F47" s="3">
         <v>10.6</v>
@@ -2071,7 +2080,7 @@
         <v>155</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F48" s="3">
         <v>12.9</v>
@@ -2094,7 +2103,7 @@
         <v>179</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F49" s="3">
         <v>11.1</v>
@@ -2117,7 +2126,7 @@
         <v>158</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F50" s="3">
         <v>12.8</v>
@@ -2140,7 +2149,7 @@
         <v>155</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F51" s="3">
         <v>9.6999999999999993</v>
@@ -2232,7 +2241,7 @@
         <v>185</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F55" s="3">
         <v>12.1</v>
@@ -2301,7 +2310,7 @@
         <v>196</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F58" s="3">
         <v>8.4</v>
@@ -2347,7 +2356,7 @@
         <v>155</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F60" s="3">
         <v>11</v>
@@ -2393,7 +2402,7 @@
         <v>145</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F62" s="3">
         <v>17.8</v>
@@ -2416,7 +2425,7 @@
         <v>160</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F63" s="3">
         <v>13</v>
@@ -2439,7 +2448,7 @@
         <v>170</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F64" s="3">
         <v>16.399999999999999</v>
@@ -2462,7 +2471,7 @@
         <v>195</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F65" s="3">
         <v>10.7</v>
@@ -2485,7 +2494,7 @@
         <v>185</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F66" s="3">
         <v>14</v>
@@ -2531,7 +2540,7 @@
         <v>142</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F68" s="3">
         <v>15.1</v>
@@ -2600,7 +2609,7 @@
         <v>175</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F71" s="3">
         <v>11.4</v>
@@ -2623,7 +2632,7 @@
         <v>160</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F72" s="3">
         <v>14.3</v>
@@ -2646,7 +2655,7 @@
         <v>187</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F73" s="3">
         <v>11.5</v>
@@ -2669,7 +2678,7 @@
         <v>160</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F74" s="3">
         <v>14.2</v>
@@ -2692,7 +2701,7 @@
         <v>175</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F75" s="3">
         <v>14.7</v>
@@ -2715,7 +2724,7 @@
         <v>190</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F76" s="3">
         <v>12.6</v>
@@ -2738,7 +2747,7 @@
         <v>230</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F77" s="3">
         <v>11.3</v>
@@ -2784,7 +2793,7 @@
         <v>145</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F79" s="3">
         <v>15.3</v>
@@ -2830,7 +2839,7 @@
         <v>145</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F81" s="3">
         <v>15</v>
@@ -2876,7 +2885,7 @@
         <v>166</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F83" s="3">
         <v>14</v>
@@ -2922,7 +2931,7 @@
         <v>145</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F85" s="3">
         <v>15.9</v>
@@ -2968,7 +2977,7 @@
         <v>145</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F87" s="3">
         <v>13.7</v>
@@ -2991,7 +3000,7 @@
         <v>195</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F88" s="3">
         <v>9.9</v>
@@ -3014,7 +3023,7 @@
         <v>165</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F89" s="3">
         <v>12.1</v>
@@ -3037,7 +3046,7 @@
         <v>205</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F90" s="3">
         <v>10.6</v>
@@ -3083,7 +3092,7 @@
         <v>155</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F92" s="3">
         <v>13.6</v>
@@ -3106,7 +3115,7 @@
         <v>152</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F93" s="3">
         <v>15.2</v>
@@ -3129,7 +3138,7 @@
         <v>160</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F94" s="3">
         <v>12.3</v>
@@ -3152,7 +3161,7 @@
         <v>141</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F95" s="3">
         <v>15.2</v>
@@ -3175,7 +3184,7 @@
         <v>183</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F96" s="3">
         <v>12.8</v>
@@ -3198,7 +3207,7 @@
         <v>163</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F97" s="3">
         <v>14.1</v>
@@ -3221,7 +3230,7 @@
         <v>205</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F98" s="3">
         <v>8.9</v>
@@ -3244,7 +3253,7 @@
         <v>134</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F99" s="3">
         <v>14.6</v>
@@ -3267,7 +3276,7 @@
         <v>155</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F100" s="3">
         <v>18.2</v>
@@ -3290,7 +3299,7 @@
         <v>152</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F101" s="3">
         <v>13.1</v>
@@ -3313,7 +3322,7 @@
         <v>152</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F102" s="3">
         <v>16.7</v>
@@ -3336,7 +3345,7 @@
         <v>150</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F103" s="3">
         <v>15</v>
@@ -3359,7 +3368,7 @@
         <v>160</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F104" s="3">
         <v>16.899999999999999</v>
@@ -3382,7 +3391,7 @@
         <v>165</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F105" s="3">
         <v>10.199999999999999</v>
@@ -3405,7 +3414,7 @@
         <v>160</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F106" s="3">
         <v>12.5</v>
@@ -3451,7 +3460,7 @@
         <v>143</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F108" s="3">
         <v>17.2</v>
@@ -3474,7 +3483,7 @@
         <v>146</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F109" s="3">
         <v>14.3</v>
@@ -3497,7 +3506,7 @@
         <v>146</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F110" s="3">
         <v>15.9</v>
@@ -3520,7 +3529,7 @@
         <v>146</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F111" s="3">
         <v>14.3</v>
@@ -3543,7 +3552,7 @@
         <v>148</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F112" s="3">
         <v>16.899999999999999</v>
@@ -3566,7 +3575,7 @@
         <v>173</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F113" s="3">
         <v>14.9</v>
@@ -3589,7 +3598,7 @@
         <v>164</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F114" s="3">
         <v>16</v>
@@ -3612,7 +3621,7 @@
         <v>182</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F115" s="3">
         <v>12.7</v>
@@ -3635,7 +3644,7 @@
         <v>155</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F116" s="3">
         <v>14</v>
@@ -3681,7 +3690,7 @@
         <v>203</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F118" s="3">
         <v>11.4</v>
@@ -3819,7 +3828,7 @@
         <v>140</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F124" s="3">
         <v>15.2</v>
@@ -3865,7 +3874,7 @@
         <v>150</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F126" s="3">
         <v>14</v>
@@ -3911,7 +3920,7 @@
         <v>145</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F128" s="3">
         <v>14</v>
@@ -4026,7 +4035,7 @@
         <v>200</v>
       </c>
       <c r="E133" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F133" s="3">
         <v>9.4</v>
@@ -4095,7 +4104,7 @@
         <v>141</v>
       </c>
       <c r="E136" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F136" s="3">
         <v>12.1</v>
@@ -4141,7 +4150,7 @@
         <v>155</v>
       </c>
       <c r="E138" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F138" s="3">
         <v>15.1</v>
@@ -4164,7 +4173,7 @@
         <v>175</v>
       </c>
       <c r="E139" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F139" s="3">
         <v>12.1</v>
@@ -4187,7 +4196,7 @@
         <v>170</v>
       </c>
       <c r="E140" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F140" s="3">
         <v>11</v>
@@ -4210,7 +4219,7 @@
         <v>170</v>
       </c>
       <c r="E141" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F141" s="3">
         <v>12.4</v>
@@ -4233,7 +4242,7 @@
         <v>170</v>
       </c>
       <c r="E142" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F142" s="3">
         <v>15</v>
@@ -4279,7 +4288,7 @@
         <v>190</v>
       </c>
       <c r="E144" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F144" s="3">
         <v>10.3</v>
@@ -4325,7 +4334,7 @@
         <v>140</v>
       </c>
       <c r="E146" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F146" s="3">
         <v>15.9</v>
@@ -4371,7 +4380,7 @@
         <v>148</v>
       </c>
       <c r="E148" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F148" s="3">
         <v>16.100000000000001</v>
@@ -4417,7 +4426,7 @@
         <v>146</v>
       </c>
       <c r="E150" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F150" s="3">
         <v>16.3</v>
@@ -4486,7 +4495,7 @@
         <v>143</v>
       </c>
       <c r="E153" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F153" s="3">
         <v>15.3</v>
@@ -4509,7 +4518,7 @@
         <v>155</v>
       </c>
       <c r="E154" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F154" s="3">
         <v>12.5</v>
@@ -4532,7 +4541,7 @@
         <v>140</v>
       </c>
       <c r="E155" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F155" s="3">
         <v>14.7</v>
@@ -4578,7 +4587,7 @@
         <v>165</v>
       </c>
       <c r="E157" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F157" s="3">
         <v>10.199999999999999</v>
@@ -4601,7 +4610,7 @@
         <v>145</v>
       </c>
       <c r="E158" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F158" s="3">
         <v>10.4</v>
@@ -4624,7 +4633,7 @@
         <v>190</v>
       </c>
       <c r="E159" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F159" s="3">
         <v>12.3</v>
@@ -4647,7 +4656,7 @@
         <v>175</v>
       </c>
       <c r="E160" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F160" s="3">
         <v>9</v>
@@ -4670,7 +4679,7 @@
         <v>155</v>
       </c>
       <c r="E161" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F161" s="3">
         <v>11.8</v>

</xml_diff>